<commit_message>
Ich bin zu faul für eine Beschreibung
</commit_message>
<xml_diff>
--- a/Protokoll.xlsx
+++ b/Protokoll.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="22">
   <si>
     <t>Datenbankmodell ausarbeiten</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Login- und Registrierungverbessreung und Design</t>
+  </si>
+  <si>
+    <t>Berwertungssystem</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +440,7 @@
     <col min="5" max="1025" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>43126</v>
       </c>
@@ -469,19 +472,31 @@
         <v>43165</v>
       </c>
       <c r="L1" s="1">
-        <v>43141</v>
+        <v>43167</v>
       </c>
       <c r="M1" s="1">
-        <v>43142</v>
+        <v>43168</v>
       </c>
       <c r="N1" s="1">
-        <v>43143</v>
+        <v>43172</v>
       </c>
       <c r="O1" s="1">
-        <v>43144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>43174</v>
+      </c>
+      <c r="P1" s="1">
+        <v>43175</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>43179</v>
+      </c>
+      <c r="R1" s="1">
+        <v>43181</v>
+      </c>
+      <c r="S1" s="1">
+        <v>43182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -489,7 +504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -497,7 +512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -505,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -513,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -527,7 +542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -541,7 +556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -549,7 +564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -557,7 +572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -568,7 +583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -584,8 +599,20 @@
       <c r="K11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -599,7 +626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -613,7 +640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -621,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -632,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -643,7 +670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -657,7 +684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -672,6 +699,23 @@
       </c>
       <c r="K18" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>8</v>
+      </c>
+      <c r="R19" t="s">
+        <v>8</v>
+      </c>
+      <c r="S19" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>